<commit_message>
Aplicacion - ABC Servicios. TODO: Usuario_Mod
</commit_message>
<xml_diff>
--- a/My Project/Archivos_Carga/Carga_Tarifas.xlsx
+++ b/My Project/Archivos_Carga/Carga_Tarifas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RESPALDO\ESCUELA\MAD - 001\PIA - Nuevo\PIA MAD\Aplicacion\PIA MAD - ScdChnc\My Project\Archivos_Carga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744326B2-47A8-44E1-AAAF-A66B90C931EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA1E2CE-58EE-4740-8CC5-6F28EBD6A760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4CBCFDA4-C8AA-47A7-8A50-858439D32C05}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Mes</t>
   </si>
@@ -409,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B26766-6072-44FE-8B21-C45C0592F3CC}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,42 +439,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1">
-        <v>120</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1">
         <v>12</v>
       </c>
       <c r="F2" s="1">
         <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2021</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aplicación - Actividad terminada. TODO: Validaciones
</commit_message>
<xml_diff>
--- a/My Project/Archivos_Carga/Carga_Tarifas.xlsx
+++ b/My Project/Archivos_Carga/Carga_Tarifas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RESPALDO\ESCUELA\MAD - 001\PIA - Nuevo\PIA MAD\Aplicacion\PIA MAD - ScdChnc\My Project\Archivos_Carga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA1E2CE-58EE-4740-8CC5-6F28EBD6A760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CF1EE9-9C45-4479-B535-A25198F9A5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4CBCFDA4-C8AA-47A7-8A50-858439D32C05}"/>
+    <workbookView xWindow="3465" yWindow="5610" windowWidth="21600" windowHeight="7080" xr2:uid="{4CBCFDA4-C8AA-47A7-8A50-858439D32C05}"/>
   </bookViews>
   <sheets>
     <sheet name="Carga_Tarifas" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
     <t>Tipo</t>
   </si>
   <si>
-    <t>I</t>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -90,10 +90,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -412,7 +415,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,23 +441,23 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
         <v>2020</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1">
-        <v>45</v>
+      <c r="D2" s="2">
+        <v>1.55</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2.81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>